<commit_message>
ajout de la fonctionnnalité d'ouverture de fichier et mise en place du graphe
</commit_message>
<xml_diff>
--- a/GPI/GANTT.xlsx
+++ b/GPI/GANTT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\iut\G4S2\SAE\GRAMA\GPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3E00355-C41A-4639-A3D5-8DBA97078DA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C64E5B-13E5-425B-B038-1C14E8C66980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{E5182A25-CAA6-4D67-9071-9F4C8FE9A0AC}"/>
+    <workbookView xWindow="9312" yWindow="2112" windowWidth="12636" windowHeight="8880" activeTab="1" xr2:uid="{E5182A25-CAA6-4D67-9071-9F4C8FE9A0AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="2" r:id="rId1"/>
@@ -1077,7 +1077,7 @@
       <selection activeCell="G1" sqref="G1"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
-      <selection pane="bottomRight" activeCell="Y20" sqref="Y20"/>
+      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
mise en place des fonctionnalités 2 et 3
</commit_message>
<xml_diff>
--- a/GPI/GANTT.xlsx
+++ b/GPI/GANTT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\iut\G4S2\SAE\GRAMA\GPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C64E5B-13E5-425B-B038-1C14E8C66980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{555D0D6C-D583-45A4-8387-897561756BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9312" yWindow="2112" windowWidth="12636" windowHeight="8880" activeTab="1" xr2:uid="{E5182A25-CAA6-4D67-9071-9F4C8FE9A0AC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{E5182A25-CAA6-4D67-9071-9F4C8FE9A0AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="2" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="119">
   <si>
     <t>WBS</t>
   </si>
@@ -492,7 +492,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -507,13 +507,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFA500"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -557,7 +551,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -619,22 +613,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1077,7 +1068,7 @@
       <selection activeCell="G1" sqref="G1"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
-      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomRight" activeCell="V8" sqref="V8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1149,7 +1140,7 @@
       <c r="N1" s="28"/>
       <c r="O1" s="28"/>
       <c r="P1" s="28"/>
-      <c r="Q1" s="32"/>
+      <c r="Q1" s="31"/>
       <c r="R1" s="27" t="s">
         <v>25</v>
       </c>
@@ -1304,7 +1295,7 @@
       <c r="N2" s="28"/>
       <c r="O2" s="28"/>
       <c r="P2" s="28"/>
-      <c r="Q2" s="32"/>
+      <c r="Q2" s="31"/>
       <c r="R2" s="27" t="s">
         <v>22</v>
       </c>
@@ -1456,7 +1447,7 @@
       <c r="P3" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="Q3" s="33" t="s">
+      <c r="Q3" s="32" t="s">
         <v>60</v>
       </c>
       <c r="R3" s="12" t="s">
@@ -1741,12 +1732,12 @@
       <c r="M4" s="18"/>
       <c r="N4" s="19"/>
       <c r="O4" s="19"/>
-      <c r="P4" s="30" t="s">
-        <v>13</v>
-      </c>
+      <c r="P4" s="19"/>
       <c r="Q4" s="19"/>
       <c r="R4" s="18"/>
-      <c r="S4" s="19"/>
+      <c r="S4" s="30" t="s">
+        <v>13</v>
+      </c>
       <c r="T4" s="19"/>
       <c r="U4" s="19"/>
       <c r="V4" s="18"/>
@@ -1857,12 +1848,12 @@
       <c r="M5" s="21"/>
       <c r="N5" s="19"/>
       <c r="O5" s="19"/>
-      <c r="P5" s="30" t="s">
-        <v>13</v>
-      </c>
+      <c r="P5" s="19"/>
       <c r="Q5" s="19"/>
       <c r="R5" s="18"/>
-      <c r="S5" s="19"/>
+      <c r="S5" s="30" t="s">
+        <v>13</v>
+      </c>
       <c r="T5" s="19"/>
       <c r="U5" s="19"/>
       <c r="V5" s="18"/>
@@ -1973,12 +1964,12 @@
       <c r="M6" s="21"/>
       <c r="N6" s="29"/>
       <c r="O6" s="19"/>
-      <c r="P6" s="30" t="s">
-        <v>13</v>
-      </c>
+      <c r="P6" s="19"/>
       <c r="Q6" s="19"/>
       <c r="R6" s="18"/>
-      <c r="S6" s="19"/>
+      <c r="S6" s="30" t="s">
+        <v>13</v>
+      </c>
       <c r="T6" s="19"/>
       <c r="U6" s="19"/>
       <c r="V6" s="18"/>
@@ -2088,12 +2079,12 @@
       <c r="M7" s="18"/>
       <c r="N7" s="29"/>
       <c r="O7" s="19"/>
-      <c r="P7" s="30" t="s">
-        <v>13</v>
-      </c>
+      <c r="P7" s="19"/>
       <c r="Q7" s="19"/>
       <c r="R7" s="18"/>
-      <c r="S7" s="19"/>
+      <c r="S7" s="30" t="s">
+        <v>13</v>
+      </c>
       <c r="T7" s="19"/>
       <c r="U7" s="19"/>
       <c r="V7" s="18"/>
@@ -2195,20 +2186,22 @@
       <c r="I8" s="25">
         <v>44638</v>
       </c>
-      <c r="J8" s="25"/>
+      <c r="J8" s="25">
+        <v>44678</v>
+      </c>
       <c r="K8" s="18"/>
       <c r="L8" s="19"/>
       <c r="M8" s="18"/>
       <c r="N8" s="19"/>
       <c r="O8" s="19"/>
-      <c r="P8" s="31" t="s">
+      <c r="P8" s="33"/>
+      <c r="Q8" s="33"/>
+      <c r="R8" s="33"/>
+      <c r="S8" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="Q8" s="19"/>
-      <c r="R8" s="18"/>
-      <c r="S8" s="19"/>
-      <c r="T8" s="19"/>
-      <c r="U8" s="19"/>
+      <c r="T8" s="33"/>
+      <c r="U8" s="33"/>
       <c r="V8" s="18"/>
       <c r="W8" s="19"/>
       <c r="X8" s="19"/>
@@ -2306,23 +2299,25 @@
         <v>108</v>
       </c>
       <c r="I9" s="25">
-        <v>44638</v>
-      </c>
-      <c r="J9" s="25"/>
+        <v>44650</v>
+      </c>
+      <c r="J9" s="25">
+        <v>44682</v>
+      </c>
       <c r="K9" s="18"/>
       <c r="L9" s="19"/>
       <c r="M9" s="18"/>
       <c r="N9" s="19"/>
       <c r="O9" s="19"/>
-      <c r="P9" s="31" t="s">
+      <c r="P9" s="19"/>
+      <c r="Q9" s="33"/>
+      <c r="R9" s="35"/>
+      <c r="S9" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="Q9" s="19"/>
-      <c r="R9" s="18"/>
-      <c r="S9" s="19"/>
-      <c r="T9" s="19"/>
-      <c r="U9" s="19"/>
-      <c r="V9" s="18"/>
+      <c r="T9" s="33"/>
+      <c r="U9" s="33"/>
+      <c r="V9" s="35"/>
       <c r="W9" s="19"/>
       <c r="X9" s="19"/>
       <c r="Y9" s="19"/>
@@ -2418,20 +2413,22 @@
       <c r="H10" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="I10" s="25"/>
+      <c r="I10" s="25">
+        <v>44671</v>
+      </c>
       <c r="J10" s="25"/>
       <c r="K10" s="18"/>
       <c r="L10" s="19"/>
       <c r="M10" s="18"/>
       <c r="N10" s="19"/>
       <c r="O10" s="19"/>
-      <c r="P10" s="30" t="s">
-        <v>13</v>
-      </c>
+      <c r="P10" s="19"/>
       <c r="Q10" s="19"/>
       <c r="R10" s="18"/>
-      <c r="S10" s="19"/>
-      <c r="T10" s="19"/>
+      <c r="S10" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="T10" s="33"/>
       <c r="U10" s="19"/>
       <c r="V10" s="18"/>
       <c r="W10" s="19"/>
@@ -2536,12 +2533,12 @@
       <c r="M11" s="18"/>
       <c r="N11" s="19"/>
       <c r="O11" s="19"/>
-      <c r="P11" s="30" t="s">
-        <v>13</v>
-      </c>
+      <c r="P11" s="19"/>
       <c r="Q11" s="19"/>
       <c r="R11" s="18"/>
-      <c r="S11" s="19"/>
+      <c r="S11" s="30" t="s">
+        <v>13</v>
+      </c>
       <c r="T11" s="19"/>
       <c r="U11" s="19"/>
       <c r="V11" s="18"/>
@@ -2647,12 +2644,12 @@
       <c r="M12" s="18"/>
       <c r="N12" s="19"/>
       <c r="O12" s="19"/>
-      <c r="P12" s="30" t="s">
-        <v>13</v>
-      </c>
+      <c r="P12" s="19"/>
       <c r="Q12" s="19"/>
       <c r="R12" s="18"/>
-      <c r="S12" s="19"/>
+      <c r="S12" s="30" t="s">
+        <v>13</v>
+      </c>
       <c r="T12" s="19"/>
       <c r="U12" s="19"/>
       <c r="V12" s="18"/>
@@ -2758,12 +2755,12 @@
       <c r="M13" s="18"/>
       <c r="N13" s="19"/>
       <c r="O13" s="19"/>
-      <c r="P13" s="30" t="s">
-        <v>13</v>
-      </c>
+      <c r="P13" s="19"/>
       <c r="Q13" s="19"/>
       <c r="R13" s="18"/>
-      <c r="S13" s="19"/>
+      <c r="S13" s="30" t="s">
+        <v>13</v>
+      </c>
       <c r="T13" s="19"/>
       <c r="U13" s="19"/>
       <c r="V13" s="18"/>
@@ -2869,12 +2866,12 @@
       <c r="M14" s="18"/>
       <c r="N14" s="19"/>
       <c r="O14" s="19"/>
-      <c r="P14" s="30" t="s">
-        <v>13</v>
-      </c>
+      <c r="P14" s="19"/>
       <c r="Q14" s="19"/>
       <c r="R14" s="18"/>
-      <c r="S14" s="19"/>
+      <c r="S14" s="30" t="s">
+        <v>13</v>
+      </c>
       <c r="T14" s="19"/>
       <c r="U14" s="19"/>
       <c r="V14" s="18"/>
@@ -2980,12 +2977,12 @@
       <c r="M15" s="18"/>
       <c r="N15" s="19"/>
       <c r="O15" s="19"/>
-      <c r="P15" s="30" t="s">
-        <v>13</v>
-      </c>
+      <c r="P15" s="19"/>
       <c r="Q15" s="19"/>
       <c r="R15" s="18"/>
-      <c r="S15" s="19"/>
+      <c r="S15" s="30" t="s">
+        <v>13</v>
+      </c>
       <c r="T15" s="19"/>
       <c r="U15" s="19"/>
       <c r="V15" s="18"/>
@@ -3091,12 +3088,12 @@
       <c r="M16" s="18"/>
       <c r="N16" s="19"/>
       <c r="O16" s="19"/>
-      <c r="P16" s="30" t="s">
-        <v>13</v>
-      </c>
+      <c r="P16" s="19"/>
       <c r="Q16" s="19"/>
       <c r="R16" s="18"/>
-      <c r="S16" s="19"/>
+      <c r="S16" s="30" t="s">
+        <v>13</v>
+      </c>
       <c r="T16" s="19"/>
       <c r="U16" s="19"/>
       <c r="V16" s="18"/>
@@ -3202,12 +3199,12 @@
       <c r="M17" s="18"/>
       <c r="N17" s="19"/>
       <c r="O17" s="19"/>
-      <c r="P17" s="30" t="s">
-        <v>13</v>
-      </c>
+      <c r="P17" s="19"/>
       <c r="Q17" s="19"/>
       <c r="R17" s="18"/>
-      <c r="S17" s="19"/>
+      <c r="S17" s="30" t="s">
+        <v>13</v>
+      </c>
       <c r="T17" s="19"/>
       <c r="U17" s="19"/>
       <c r="V17" s="18"/>
@@ -3313,12 +3310,12 @@
       <c r="M18" s="18"/>
       <c r="N18" s="19"/>
       <c r="O18" s="19"/>
-      <c r="P18" s="30" t="s">
-        <v>13</v>
-      </c>
+      <c r="P18" s="19"/>
       <c r="Q18" s="19"/>
       <c r="R18" s="18"/>
-      <c r="S18" s="19"/>
+      <c r="S18" s="30" t="s">
+        <v>13</v>
+      </c>
       <c r="T18" s="19"/>
       <c r="U18" s="19"/>
       <c r="V18" s="18"/>
@@ -3424,12 +3421,12 @@
       <c r="M19" s="18"/>
       <c r="N19" s="19"/>
       <c r="O19" s="19"/>
-      <c r="P19" s="30" t="s">
-        <v>13</v>
-      </c>
+      <c r="P19" s="19"/>
       <c r="Q19" s="19"/>
       <c r="R19" s="18"/>
-      <c r="S19" s="19"/>
+      <c r="S19" s="30" t="s">
+        <v>13</v>
+      </c>
       <c r="T19" s="19"/>
       <c r="U19" s="19"/>
       <c r="V19" s="18"/>
@@ -3537,21 +3534,21 @@
       <c r="K20" s="18"/>
       <c r="L20" s="19"/>
       <c r="M20" s="18"/>
-      <c r="N20" s="34"/>
-      <c r="O20" s="34"/>
-      <c r="P20" s="35" t="s">
+      <c r="N20" s="33"/>
+      <c r="O20" s="33"/>
+      <c r="P20" s="33"/>
+      <c r="Q20" s="33"/>
+      <c r="R20" s="35"/>
+      <c r="S20" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="Q20" s="34"/>
-      <c r="R20" s="36"/>
-      <c r="S20" s="34"/>
-      <c r="T20" s="34"/>
-      <c r="U20" s="34"/>
-      <c r="V20" s="36"/>
-      <c r="W20" s="34"/>
-      <c r="X20" s="34"/>
-      <c r="Y20" s="34"/>
-      <c r="Z20" s="36"/>
+      <c r="T20" s="33"/>
+      <c r="U20" s="33"/>
+      <c r="V20" s="35"/>
+      <c r="W20" s="33"/>
+      <c r="X20" s="33"/>
+      <c r="Y20" s="33"/>
+      <c r="Z20" s="35"/>
       <c r="AA20" s="19"/>
       <c r="AB20" s="19"/>
       <c r="AC20" s="19"/>
@@ -3635,99 +3632,6 @@
       <c r="D21" s="25"/>
       <c r="E21" s="25"/>
       <c r="F21" s="26"/>
-      <c r="K21" s="18"/>
-      <c r="L21" s="19"/>
-      <c r="M21" s="18"/>
-      <c r="N21" s="19"/>
-      <c r="O21" s="19"/>
-      <c r="P21" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q21" s="19"/>
-      <c r="R21" s="18"/>
-      <c r="S21" s="19"/>
-      <c r="T21" s="19"/>
-      <c r="U21" s="19"/>
-      <c r="V21" s="18"/>
-      <c r="W21" s="19"/>
-      <c r="X21" s="19"/>
-      <c r="Y21" s="19"/>
-      <c r="Z21" s="18"/>
-      <c r="AA21" s="19"/>
-      <c r="AB21" s="19"/>
-      <c r="AC21" s="19"/>
-      <c r="AD21" s="19"/>
-      <c r="AE21" s="18"/>
-      <c r="AF21" s="19"/>
-      <c r="AG21" s="19"/>
-      <c r="AH21" s="19"/>
-      <c r="AI21" s="18"/>
-      <c r="AJ21" s="19"/>
-      <c r="AK21" s="19"/>
-      <c r="AL21" s="19"/>
-      <c r="AM21" s="18"/>
-      <c r="AN21" s="19"/>
-      <c r="AO21" s="19"/>
-      <c r="AP21" s="19"/>
-      <c r="AQ21" s="19"/>
-      <c r="AR21" s="18"/>
-      <c r="AS21" s="19"/>
-      <c r="AT21" s="19"/>
-      <c r="AU21" s="19"/>
-      <c r="AV21" s="18"/>
-      <c r="AW21" s="19"/>
-      <c r="AX21" s="19"/>
-      <c r="AY21" s="19"/>
-      <c r="AZ21" s="18"/>
-      <c r="BA21" s="19"/>
-      <c r="BB21" s="19"/>
-      <c r="BC21" s="19"/>
-      <c r="BD21" s="19"/>
-      <c r="BE21" s="18"/>
-      <c r="BF21" s="19"/>
-      <c r="BG21" s="19"/>
-      <c r="BH21" s="19"/>
-      <c r="BI21" s="18"/>
-      <c r="BJ21" s="19"/>
-      <c r="BK21" s="19"/>
-      <c r="BL21" s="19"/>
-      <c r="BM21" s="18"/>
-      <c r="BN21" s="19"/>
-      <c r="BO21" s="19"/>
-      <c r="BP21" s="19"/>
-      <c r="BQ21" s="19"/>
-      <c r="BR21" s="18"/>
-      <c r="BS21" s="19"/>
-      <c r="BT21" s="19"/>
-      <c r="BU21" s="19"/>
-      <c r="BV21" s="18"/>
-      <c r="BW21" s="19"/>
-      <c r="BX21" s="19"/>
-      <c r="BY21" s="19"/>
-      <c r="BZ21" s="18"/>
-      <c r="CA21" s="19"/>
-      <c r="CB21" s="19"/>
-      <c r="CC21" s="19"/>
-      <c r="CD21" s="19"/>
-      <c r="CE21" s="18"/>
-      <c r="CF21" s="19"/>
-      <c r="CG21" s="19"/>
-      <c r="CH21" s="19"/>
-      <c r="CI21" s="18"/>
-      <c r="CJ21" s="19"/>
-      <c r="CK21" s="19"/>
-      <c r="CL21" s="19"/>
-      <c r="CM21" s="19"/>
-      <c r="CN21" s="18"/>
-      <c r="CO21" s="19"/>
-      <c r="CP21" s="19"/>
-      <c r="CQ21" s="19"/>
-      <c r="CR21" s="18"/>
-      <c r="CS21" s="19"/>
-      <c r="CT21" s="19"/>
-      <c r="CU21" s="19"/>
-      <c r="CV21" s="18"/>
-      <c r="CW21" s="19"/>
     </row>
     <row r="22" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A22" s="23"/>

</xml_diff>

<commit_message>
suite de la jframe
</commit_message>
<xml_diff>
--- a/GPI/GANTT.xlsx
+++ b/GPI/GANTT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\iut\G4S2\SAE\GRAMA\GPI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\iut\G4S2\SAE\GRAMA - git\GPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16693988-6A53-4089-9C41-97A2C641A311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9ECF8CD-260B-4B3E-AD22-567FA02FBC41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{E5182A25-CAA6-4D67-9071-9F4C8FE9A0AC}"/>
+    <workbookView xWindow="2124" yWindow="2124" windowWidth="12636" windowHeight="8880" activeTab="1" xr2:uid="{E5182A25-CAA6-4D67-9071-9F4C8FE9A0AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="2" r:id="rId1"/>
@@ -507,7 +507,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFA500"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -551,7 +551,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -619,10 +619,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -939,7 +942,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="438" row="0">
+  <wetp:taskpane dockstate="right" visibility="0" width="172" row="0">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -970,7 +973,7 @@
   <dimension ref="B2:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1016,7 +1019,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="7">
-        <v>44683</v>
+        <v>44732</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.3">
@@ -1735,13 +1738,13 @@
       <c r="S4" s="19"/>
       <c r="T4" s="19"/>
       <c r="U4" s="19"/>
-      <c r="V4" s="32" t="s">
-        <v>13</v>
-      </c>
+      <c r="V4" s="18"/>
       <c r="W4" s="19"/>
       <c r="X4" s="19"/>
       <c r="Y4" s="19"/>
-      <c r="Z4" s="18"/>
+      <c r="Z4" s="32" t="s">
+        <v>13</v>
+      </c>
       <c r="AA4" s="19"/>
       <c r="AB4" s="19"/>
       <c r="AC4" s="19"/>
@@ -1851,13 +1854,13 @@
       <c r="S5" s="19"/>
       <c r="T5" s="19"/>
       <c r="U5" s="19"/>
-      <c r="V5" s="32" t="s">
-        <v>13</v>
-      </c>
+      <c r="V5" s="18"/>
       <c r="W5" s="19"/>
       <c r="X5" s="19"/>
       <c r="Y5" s="19"/>
-      <c r="Z5" s="18"/>
+      <c r="Z5" s="32" t="s">
+        <v>13</v>
+      </c>
       <c r="AA5" s="19"/>
       <c r="AB5" s="19"/>
       <c r="AC5" s="19"/>
@@ -1967,13 +1970,13 @@
       <c r="S6" s="19"/>
       <c r="T6" s="19"/>
       <c r="U6" s="19"/>
-      <c r="V6" s="32" t="s">
-        <v>13</v>
-      </c>
+      <c r="V6" s="18"/>
       <c r="W6" s="19"/>
       <c r="X6" s="19"/>
       <c r="Y6" s="19"/>
-      <c r="Z6" s="18"/>
+      <c r="Z6" s="32" t="s">
+        <v>13</v>
+      </c>
       <c r="AA6" s="19"/>
       <c r="AB6" s="19"/>
       <c r="AC6" s="19"/>
@@ -2082,13 +2085,13 @@
       <c r="S7" s="19"/>
       <c r="T7" s="19"/>
       <c r="U7" s="19"/>
-      <c r="V7" s="32" t="s">
-        <v>13</v>
-      </c>
+      <c r="V7" s="18"/>
       <c r="W7" s="19"/>
       <c r="X7" s="19"/>
       <c r="Y7" s="19"/>
-      <c r="Z7" s="18"/>
+      <c r="Z7" s="32" t="s">
+        <v>13</v>
+      </c>
       <c r="AA7" s="19"/>
       <c r="AB7" s="19"/>
       <c r="AC7" s="19"/>
@@ -2197,13 +2200,13 @@
       <c r="S8" s="29"/>
       <c r="T8" s="29"/>
       <c r="U8" s="29"/>
-      <c r="V8" s="32" t="s">
-        <v>13</v>
-      </c>
+      <c r="V8" s="18"/>
       <c r="W8" s="19"/>
       <c r="X8" s="19"/>
       <c r="Y8" s="19"/>
-      <c r="Z8" s="18"/>
+      <c r="Z8" s="32" t="s">
+        <v>13</v>
+      </c>
       <c r="AA8" s="19"/>
       <c r="AB8" s="19"/>
       <c r="AC8" s="19"/>
@@ -2312,13 +2315,13 @@
       <c r="S9" s="29"/>
       <c r="T9" s="29"/>
       <c r="U9" s="29"/>
-      <c r="V9" s="33" t="s">
-        <v>13</v>
-      </c>
+      <c r="V9" s="21"/>
       <c r="W9" s="19"/>
       <c r="X9" s="19"/>
       <c r="Y9" s="19"/>
-      <c r="Z9" s="18"/>
+      <c r="Z9" s="32" t="s">
+        <v>13</v>
+      </c>
       <c r="AA9" s="19"/>
       <c r="AB9" s="19"/>
       <c r="AC9" s="19"/>
@@ -2427,13 +2430,13 @@
       <c r="S10" s="19"/>
       <c r="T10" s="29"/>
       <c r="U10" s="29"/>
-      <c r="V10" s="33" t="s">
-        <v>13</v>
-      </c>
+      <c r="V10" s="21"/>
       <c r="W10" s="19"/>
       <c r="X10" s="19"/>
       <c r="Y10" s="19"/>
-      <c r="Z10" s="18"/>
+      <c r="Z10" s="32" t="s">
+        <v>13</v>
+      </c>
       <c r="AA10" s="19"/>
       <c r="AB10" s="19"/>
       <c r="AC10" s="19"/>
@@ -2538,13 +2541,13 @@
       <c r="S11" s="19"/>
       <c r="T11" s="19"/>
       <c r="U11" s="19"/>
-      <c r="V11" s="32" t="s">
-        <v>13</v>
-      </c>
+      <c r="V11" s="18"/>
       <c r="W11" s="19"/>
       <c r="X11" s="19"/>
       <c r="Y11" s="19"/>
-      <c r="Z11" s="18"/>
+      <c r="Z11" s="32" t="s">
+        <v>13</v>
+      </c>
       <c r="AA11" s="19"/>
       <c r="AB11" s="19"/>
       <c r="AC11" s="19"/>
@@ -2649,13 +2652,13 @@
       <c r="S12" s="19"/>
       <c r="T12" s="19"/>
       <c r="U12" s="19"/>
-      <c r="V12" s="32" t="s">
-        <v>13</v>
-      </c>
+      <c r="V12" s="18"/>
       <c r="W12" s="19"/>
       <c r="X12" s="19"/>
       <c r="Y12" s="19"/>
-      <c r="Z12" s="18"/>
+      <c r="Z12" s="32" t="s">
+        <v>13</v>
+      </c>
       <c r="AA12" s="19"/>
       <c r="AB12" s="19"/>
       <c r="AC12" s="19"/>
@@ -2760,13 +2763,13 @@
       <c r="S13" s="19"/>
       <c r="T13" s="19"/>
       <c r="U13" s="19"/>
-      <c r="V13" s="32" t="s">
-        <v>13</v>
-      </c>
+      <c r="V13" s="18"/>
       <c r="W13" s="19"/>
       <c r="X13" s="19"/>
       <c r="Y13" s="19"/>
-      <c r="Z13" s="18"/>
+      <c r="Z13" s="32" t="s">
+        <v>13</v>
+      </c>
       <c r="AA13" s="19"/>
       <c r="AB13" s="19"/>
       <c r="AC13" s="19"/>
@@ -2871,13 +2874,13 @@
       <c r="S14" s="19"/>
       <c r="T14" s="19"/>
       <c r="U14" s="19"/>
-      <c r="V14" s="32" t="s">
-        <v>13</v>
-      </c>
+      <c r="V14" s="18"/>
       <c r="W14" s="19"/>
       <c r="X14" s="19"/>
       <c r="Y14" s="19"/>
-      <c r="Z14" s="18"/>
+      <c r="Z14" s="32" t="s">
+        <v>13</v>
+      </c>
       <c r="AA14" s="19"/>
       <c r="AB14" s="19"/>
       <c r="AC14" s="19"/>
@@ -2982,13 +2985,13 @@
       <c r="S15" s="19"/>
       <c r="T15" s="19"/>
       <c r="U15" s="19"/>
-      <c r="V15" s="32" t="s">
-        <v>13</v>
-      </c>
+      <c r="V15" s="18"/>
       <c r="W15" s="19"/>
       <c r="X15" s="19"/>
       <c r="Y15" s="19"/>
-      <c r="Z15" s="18"/>
+      <c r="Z15" s="32" t="s">
+        <v>13</v>
+      </c>
       <c r="AA15" s="19"/>
       <c r="AB15" s="19"/>
       <c r="AC15" s="19"/>
@@ -3093,13 +3096,13 @@
       <c r="S16" s="19"/>
       <c r="T16" s="19"/>
       <c r="U16" s="19"/>
-      <c r="V16" s="32" t="s">
-        <v>13</v>
-      </c>
+      <c r="V16" s="18"/>
       <c r="W16" s="19"/>
       <c r="X16" s="19"/>
       <c r="Y16" s="19"/>
-      <c r="Z16" s="18"/>
+      <c r="Z16" s="32" t="s">
+        <v>13</v>
+      </c>
       <c r="AA16" s="19"/>
       <c r="AB16" s="19"/>
       <c r="AC16" s="19"/>
@@ -3204,13 +3207,13 @@
       <c r="S17" s="19"/>
       <c r="T17" s="19"/>
       <c r="U17" s="19"/>
-      <c r="V17" s="32" t="s">
-        <v>13</v>
-      </c>
+      <c r="V17" s="18"/>
       <c r="W17" s="19"/>
       <c r="X17" s="19"/>
       <c r="Y17" s="19"/>
-      <c r="Z17" s="18"/>
+      <c r="Z17" s="32" t="s">
+        <v>13</v>
+      </c>
       <c r="AA17" s="19"/>
       <c r="AB17" s="19"/>
       <c r="AC17" s="19"/>
@@ -3315,13 +3318,13 @@
       <c r="S18" s="19"/>
       <c r="T18" s="19"/>
       <c r="U18" s="19"/>
-      <c r="V18" s="32" t="s">
-        <v>13</v>
-      </c>
+      <c r="V18" s="18"/>
       <c r="W18" s="19"/>
       <c r="X18" s="19"/>
       <c r="Y18" s="19"/>
-      <c r="Z18" s="18"/>
+      <c r="Z18" s="32" t="s">
+        <v>13</v>
+      </c>
       <c r="AA18" s="19"/>
       <c r="AB18" s="19"/>
       <c r="AC18" s="19"/>
@@ -3426,13 +3429,13 @@
       <c r="S19" s="19"/>
       <c r="T19" s="19"/>
       <c r="U19" s="19"/>
-      <c r="V19" s="32" t="s">
-        <v>13</v>
-      </c>
+      <c r="V19" s="18"/>
       <c r="W19" s="19"/>
       <c r="X19" s="19"/>
       <c r="Y19" s="19"/>
-      <c r="Z19" s="18"/>
+      <c r="Z19" s="32" t="s">
+        <v>13</v>
+      </c>
       <c r="AA19" s="19"/>
       <c r="AB19" s="19"/>
       <c r="AC19" s="19"/>
@@ -3527,28 +3530,30 @@
       <c r="I20" s="25">
         <v>44627</v>
       </c>
-      <c r="J20" s="25"/>
+      <c r="J20" s="25">
+        <v>44732</v>
+      </c>
       <c r="K20" s="18"/>
       <c r="L20" s="19"/>
       <c r="M20" s="18"/>
-      <c r="N20" s="34"/>
-      <c r="O20" s="19"/>
-      <c r="P20" s="19"/>
-      <c r="Q20" s="19"/>
-      <c r="R20" s="18"/>
-      <c r="S20" s="19"/>
-      <c r="T20" s="19"/>
-      <c r="U20" s="19"/>
-      <c r="V20" s="32" t="s">
+      <c r="N20" s="33"/>
+      <c r="O20" s="33"/>
+      <c r="P20" s="33"/>
+      <c r="Q20" s="33"/>
+      <c r="R20" s="34"/>
+      <c r="S20" s="33"/>
+      <c r="T20" s="33"/>
+      <c r="U20" s="33"/>
+      <c r="V20" s="34"/>
+      <c r="W20" s="33"/>
+      <c r="X20" s="33"/>
+      <c r="Y20" s="33"/>
+      <c r="Z20" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="W20" s="19"/>
-      <c r="X20" s="19"/>
-      <c r="Y20" s="19"/>
-      <c r="Z20" s="18"/>
-      <c r="AA20" s="19"/>
-      <c r="AB20" s="19"/>
-      <c r="AC20" s="19"/>
+      <c r="AA20" s="33"/>
+      <c r="AB20" s="33"/>
+      <c r="AC20" s="33"/>
       <c r="AD20" s="19"/>
       <c r="AE20" s="18"/>
       <c r="AF20" s="19"/>

</xml_diff>

<commit_message>
écran 2 et 3 + fonctionnalité 4
</commit_message>
<xml_diff>
--- a/GPI/GANTT.xlsx
+++ b/GPI/GANTT.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\iut\G4S2\SAE\GRAMA - git\GPI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\iut\G4S2\SAE\GRAMA\GPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9ECF8CD-260B-4B3E-AD22-567FA02FBC41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73FABCCC-16E2-4DFE-B1D3-D86616D16773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2124" yWindow="2124" windowWidth="12636" windowHeight="8880" activeTab="1" xr2:uid="{E5182A25-CAA6-4D67-9071-9F4C8FE9A0AC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{E5182A25-CAA6-4D67-9071-9F4C8FE9A0AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="2" r:id="rId1"/>
@@ -492,7 +492,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -508,6 +508,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFA500"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -551,7 +557,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -626,6 +632,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -942,7 +954,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="172" row="0">
+  <wetp:taskpane dockstate="right" visibility="0" width="438" row="0">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -1068,7 +1080,7 @@
       <selection activeCell="G1" sqref="G1"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
-      <selection pane="bottomRight" activeCell="J21" sqref="J21"/>
+      <selection pane="bottomRight" activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2528,8 +2540,12 @@
       <c r="H11" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
+      <c r="I11" s="25">
+        <v>44684</v>
+      </c>
+      <c r="J11" s="25">
+        <v>44686</v>
+      </c>
       <c r="K11" s="18"/>
       <c r="L11" s="19"/>
       <c r="M11" s="18"/>
@@ -2541,7 +2557,7 @@
       <c r="S11" s="19"/>
       <c r="T11" s="19"/>
       <c r="U11" s="19"/>
-      <c r="V11" s="18"/>
+      <c r="V11" s="21"/>
       <c r="W11" s="19"/>
       <c r="X11" s="19"/>
       <c r="Y11" s="19"/>
@@ -2639,8 +2655,12 @@
       <c r="H12" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
+      <c r="I12" s="25">
+        <v>44697</v>
+      </c>
+      <c r="J12" s="25">
+        <v>44697</v>
+      </c>
       <c r="K12" s="18"/>
       <c r="L12" s="19"/>
       <c r="M12" s="18"/>
@@ -2654,7 +2674,7 @@
       <c r="U12" s="19"/>
       <c r="V12" s="18"/>
       <c r="W12" s="19"/>
-      <c r="X12" s="19"/>
+      <c r="X12" s="29"/>
       <c r="Y12" s="19"/>
       <c r="Z12" s="32" t="s">
         <v>13</v>
@@ -2750,7 +2770,9 @@
       <c r="H13" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="I13" s="25"/>
+      <c r="I13" s="25">
+        <v>44698</v>
+      </c>
       <c r="J13" s="25"/>
       <c r="K13" s="18"/>
       <c r="L13" s="19"/>
@@ -2765,7 +2787,7 @@
       <c r="U13" s="19"/>
       <c r="V13" s="18"/>
       <c r="W13" s="19"/>
-      <c r="X13" s="19"/>
+      <c r="X13" s="36"/>
       <c r="Y13" s="19"/>
       <c r="Z13" s="32" t="s">
         <v>13</v>
@@ -2861,8 +2883,12 @@
       <c r="H14" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
+      <c r="I14" s="25">
+        <v>44701</v>
+      </c>
+      <c r="J14" s="25">
+        <v>44716</v>
+      </c>
       <c r="K14" s="18"/>
       <c r="L14" s="19"/>
       <c r="M14" s="18"/>
@@ -2877,11 +2903,11 @@
       <c r="V14" s="18"/>
       <c r="W14" s="19"/>
       <c r="X14" s="19"/>
-      <c r="Y14" s="19"/>
-      <c r="Z14" s="32" t="s">
+      <c r="Y14" s="29"/>
+      <c r="Z14" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="AA14" s="19"/>
+      <c r="AA14" s="29"/>
       <c r="AB14" s="19"/>
       <c r="AC14" s="19"/>
       <c r="AD14" s="19"/>
@@ -2972,8 +2998,12 @@
       <c r="H15" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
+      <c r="I15" s="25">
+        <v>44714</v>
+      </c>
+      <c r="J15" s="25">
+        <v>44716</v>
+      </c>
       <c r="K15" s="18"/>
       <c r="L15" s="19"/>
       <c r="M15" s="18"/>
@@ -2989,10 +3019,10 @@
       <c r="W15" s="19"/>
       <c r="X15" s="19"/>
       <c r="Y15" s="19"/>
-      <c r="Z15" s="32" t="s">
+      <c r="Z15" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="AA15" s="19"/>
+      <c r="AA15" s="29"/>
       <c r="AB15" s="19"/>
       <c r="AC15" s="19"/>
       <c r="AD15" s="19"/>
@@ -3083,7 +3113,9 @@
       <c r="H16" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="I16" s="25"/>
+      <c r="I16" s="25">
+        <v>44704</v>
+      </c>
       <c r="J16" s="25"/>
       <c r="K16" s="18"/>
       <c r="L16" s="19"/>
@@ -3099,7 +3131,7 @@
       <c r="V16" s="18"/>
       <c r="W16" s="19"/>
       <c r="X16" s="19"/>
-      <c r="Y16" s="19"/>
+      <c r="Y16" s="36"/>
       <c r="Z16" s="32" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
modification du dessin du graphe
</commit_message>
<xml_diff>
--- a/GPI/GANTT.xlsx
+++ b/GPI/GANTT.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\iut\G4S2\SAE\GRAMA\GPI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\iut\G4S2\SAE\GRAMA - git\GPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73FABCCC-16E2-4DFE-B1D3-D86616D16773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D3E935-3424-4E89-912D-7DFF851CC332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{E5182A25-CAA6-4D67-9071-9F4C8FE9A0AC}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="117">
   <si>
     <t>WBS</t>
   </si>
@@ -410,12 +410,6 @@
   </si>
   <si>
     <t>Document de spécification technique</t>
-  </si>
-  <si>
-    <t>Fonctionnalité 5 (BONUS)</t>
-  </si>
-  <si>
-    <t>Réalisation de l'écran 4 de l'application (BONUS)</t>
   </si>
 </sst>
 </file>
@@ -492,7 +486,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -507,18 +501,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFA500"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -553,11 +541,137 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -599,9 +713,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -613,31 +724,64 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1031,7 +1175,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="7">
-        <v>44732</v>
+        <v>44728</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.3">
@@ -1046,7 +1190,7 @@
       <c r="B11" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="22">
+      <c r="C11" s="21">
         <v>0</v>
       </c>
     </row>
@@ -1080,7 +1224,7 @@
       <selection activeCell="G1" sqref="G1"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
-      <selection pane="bottomRight" activeCell="J15" sqref="J15"/>
+      <selection pane="bottomRight" activeCell="Y5" sqref="Y5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1144,139 +1288,139 @@
       <c r="E1" s="4"/>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="27" t="s">
+      <c r="K1" s="26"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="27" t="s">
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="27" t="s">
+      <c r="S1" s="27"/>
+      <c r="T1" s="27"/>
+      <c r="U1" s="27"/>
+      <c r="V1" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="W1" s="28"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="28"/>
-      <c r="Z1" s="27" t="s">
+      <c r="W1" s="27"/>
+      <c r="X1" s="27"/>
+      <c r="Y1" s="27"/>
+      <c r="Z1" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="AA1" s="28"/>
-      <c r="AB1" s="28"/>
-      <c r="AC1" s="28"/>
-      <c r="AD1" s="28"/>
-      <c r="AE1" s="27" t="s">
+      <c r="AA1" s="27"/>
+      <c r="AB1" s="27"/>
+      <c r="AC1" s="27"/>
+      <c r="AD1" s="27"/>
+      <c r="AE1" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="AF1" s="28"/>
-      <c r="AG1" s="28"/>
-      <c r="AH1" s="28"/>
-      <c r="AI1" s="27" t="s">
+      <c r="AF1" s="27"/>
+      <c r="AG1" s="27"/>
+      <c r="AH1" s="27"/>
+      <c r="AI1" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="AJ1" s="28"/>
-      <c r="AK1" s="28"/>
-      <c r="AL1" s="28"/>
-      <c r="AM1" s="27" t="s">
+      <c r="AJ1" s="27"/>
+      <c r="AK1" s="27"/>
+      <c r="AL1" s="27"/>
+      <c r="AM1" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="AN1" s="28"/>
-      <c r="AO1" s="28"/>
-      <c r="AP1" s="28"/>
-      <c r="AQ1" s="28"/>
-      <c r="AR1" s="27" t="s">
+      <c r="AN1" s="27"/>
+      <c r="AO1" s="27"/>
+      <c r="AP1" s="27"/>
+      <c r="AQ1" s="27"/>
+      <c r="AR1" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="AS1" s="28"/>
-      <c r="AT1" s="28"/>
-      <c r="AU1" s="28"/>
-      <c r="AV1" s="27" t="s">
+      <c r="AS1" s="27"/>
+      <c r="AT1" s="27"/>
+      <c r="AU1" s="27"/>
+      <c r="AV1" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="AW1" s="28"/>
-      <c r="AX1" s="28"/>
-      <c r="AY1" s="28"/>
-      <c r="AZ1" s="27" t="s">
+      <c r="AW1" s="27"/>
+      <c r="AX1" s="27"/>
+      <c r="AY1" s="27"/>
+      <c r="AZ1" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="BA1" s="28"/>
-      <c r="BB1" s="28"/>
-      <c r="BC1" s="28"/>
-      <c r="BD1" s="28"/>
-      <c r="BE1" s="27" t="s">
+      <c r="BA1" s="27"/>
+      <c r="BB1" s="27"/>
+      <c r="BC1" s="27"/>
+      <c r="BD1" s="27"/>
+      <c r="BE1" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="BF1" s="28"/>
-      <c r="BG1" s="28"/>
-      <c r="BH1" s="28"/>
-      <c r="BI1" s="27" t="s">
+      <c r="BF1" s="27"/>
+      <c r="BG1" s="27"/>
+      <c r="BH1" s="27"/>
+      <c r="BI1" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="BJ1" s="28"/>
-      <c r="BK1" s="28"/>
-      <c r="BL1" s="28"/>
-      <c r="BM1" s="27" t="s">
+      <c r="BJ1" s="27"/>
+      <c r="BK1" s="27"/>
+      <c r="BL1" s="27"/>
+      <c r="BM1" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="BN1" s="28"/>
-      <c r="BO1" s="28"/>
-      <c r="BP1" s="28"/>
-      <c r="BQ1" s="28"/>
-      <c r="BR1" s="27" t="s">
+      <c r="BN1" s="27"/>
+      <c r="BO1" s="27"/>
+      <c r="BP1" s="27"/>
+      <c r="BQ1" s="27"/>
+      <c r="BR1" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="BS1" s="28"/>
-      <c r="BT1" s="28"/>
-      <c r="BU1" s="28"/>
-      <c r="BV1" s="27" t="s">
+      <c r="BS1" s="27"/>
+      <c r="BT1" s="27"/>
+      <c r="BU1" s="27"/>
+      <c r="BV1" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="BW1" s="28"/>
-      <c r="BX1" s="28"/>
-      <c r="BY1" s="28"/>
-      <c r="BZ1" s="27" t="s">
+      <c r="BW1" s="27"/>
+      <c r="BX1" s="27"/>
+      <c r="BY1" s="27"/>
+      <c r="BZ1" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="CA1" s="28"/>
-      <c r="CB1" s="28"/>
-      <c r="CC1" s="28"/>
-      <c r="CD1" s="28"/>
-      <c r="CE1" s="27" t="s">
+      <c r="CA1" s="27"/>
+      <c r="CB1" s="27"/>
+      <c r="CC1" s="27"/>
+      <c r="CD1" s="27"/>
+      <c r="CE1" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="CF1" s="28"/>
-      <c r="CG1" s="28"/>
-      <c r="CH1" s="28"/>
-      <c r="CI1" s="27" t="s">
+      <c r="CF1" s="27"/>
+      <c r="CG1" s="27"/>
+      <c r="CH1" s="27"/>
+      <c r="CI1" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="CJ1" s="28"/>
-      <c r="CK1" s="28"/>
-      <c r="CL1" s="28"/>
-      <c r="CM1" s="28"/>
-      <c r="CN1" s="27" t="s">
+      <c r="CJ1" s="27"/>
+      <c r="CK1" s="27"/>
+      <c r="CL1" s="27"/>
+      <c r="CM1" s="27"/>
+      <c r="CN1" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="CO1" s="28"/>
-      <c r="CP1" s="28"/>
-      <c r="CQ1" s="28"/>
-      <c r="CR1" s="27" t="s">
+      <c r="CO1" s="27"/>
+      <c r="CP1" s="27"/>
+      <c r="CQ1" s="27"/>
+      <c r="CR1" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="CS1" s="28"/>
-      <c r="CT1" s="28"/>
-      <c r="CU1" s="28"/>
-      <c r="CV1" s="27" t="s">
+      <c r="CS1" s="27"/>
+      <c r="CT1" s="27"/>
+      <c r="CU1" s="27"/>
+      <c r="CV1" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="CW1" s="28"/>
+      <c r="CW1" s="27"/>
       <c r="CX1" s="17"/>
     </row>
     <row r="2" spans="1:102" x14ac:dyDescent="0.3">
@@ -1299,144 +1443,144 @@
       <c r="J2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="27"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="27" t="s">
+      <c r="K2" s="26"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
-      <c r="P2" s="28"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="27" t="s">
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="28"/>
+      <c r="R2" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="S2" s="28"/>
-      <c r="T2" s="28"/>
-      <c r="U2" s="28"/>
-      <c r="V2" s="27" t="s">
+      <c r="S2" s="27"/>
+      <c r="T2" s="27"/>
+      <c r="U2" s="27"/>
+      <c r="V2" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="W2" s="28"/>
-      <c r="X2" s="28"/>
-      <c r="Y2" s="28"/>
-      <c r="Z2" s="27" t="s">
+      <c r="W2" s="27"/>
+      <c r="X2" s="27"/>
+      <c r="Y2" s="27"/>
+      <c r="Z2" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="AA2" s="28"/>
-      <c r="AB2" s="28"/>
-      <c r="AC2" s="28"/>
-      <c r="AD2" s="28"/>
-      <c r="AE2" s="27" t="s">
+      <c r="AA2" s="27"/>
+      <c r="AB2" s="27"/>
+      <c r="AC2" s="27"/>
+      <c r="AD2" s="27"/>
+      <c r="AE2" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="AF2" s="28"/>
-      <c r="AG2" s="28"/>
-      <c r="AH2" s="28"/>
-      <c r="AI2" s="27" t="s">
+      <c r="AF2" s="27"/>
+      <c r="AG2" s="27"/>
+      <c r="AH2" s="27"/>
+      <c r="AI2" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="AJ2" s="28"/>
-      <c r="AK2" s="28"/>
-      <c r="AL2" s="28"/>
-      <c r="AM2" s="27" t="s">
+      <c r="AJ2" s="27"/>
+      <c r="AK2" s="27"/>
+      <c r="AL2" s="27"/>
+      <c r="AM2" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="AN2" s="28"/>
-      <c r="AO2" s="28"/>
-      <c r="AP2" s="28"/>
-      <c r="AQ2" s="28"/>
-      <c r="AR2" s="27" t="s">
+      <c r="AN2" s="27"/>
+      <c r="AO2" s="27"/>
+      <c r="AP2" s="27"/>
+      <c r="AQ2" s="27"/>
+      <c r="AR2" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="AS2" s="28"/>
-      <c r="AT2" s="28"/>
-      <c r="AU2" s="28"/>
-      <c r="AV2" s="27" t="s">
+      <c r="AS2" s="27"/>
+      <c r="AT2" s="27"/>
+      <c r="AU2" s="27"/>
+      <c r="AV2" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="AW2" s="28"/>
-      <c r="AX2" s="28"/>
-      <c r="AY2" s="28"/>
-      <c r="AZ2" s="27" t="s">
+      <c r="AW2" s="27"/>
+      <c r="AX2" s="27"/>
+      <c r="AY2" s="27"/>
+      <c r="AZ2" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="BA2" s="28"/>
-      <c r="BB2" s="28"/>
-      <c r="BC2" s="28"/>
-      <c r="BD2" s="28"/>
-      <c r="BE2" s="27" t="s">
+      <c r="BA2" s="27"/>
+      <c r="BB2" s="27"/>
+      <c r="BC2" s="27"/>
+      <c r="BD2" s="27"/>
+      <c r="BE2" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="BF2" s="28"/>
-      <c r="BG2" s="28"/>
-      <c r="BH2" s="28"/>
-      <c r="BI2" s="27" t="s">
+      <c r="BF2" s="27"/>
+      <c r="BG2" s="27"/>
+      <c r="BH2" s="27"/>
+      <c r="BI2" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="BJ2" s="28"/>
-      <c r="BK2" s="28"/>
-      <c r="BL2" s="28"/>
-      <c r="BM2" s="27" t="s">
+      <c r="BJ2" s="27"/>
+      <c r="BK2" s="27"/>
+      <c r="BL2" s="27"/>
+      <c r="BM2" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="BN2" s="28"/>
-      <c r="BO2" s="28"/>
-      <c r="BP2" s="28"/>
-      <c r="BQ2" s="28"/>
-      <c r="BR2" s="27" t="s">
+      <c r="BN2" s="27"/>
+      <c r="BO2" s="27"/>
+      <c r="BP2" s="27"/>
+      <c r="BQ2" s="27"/>
+      <c r="BR2" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="BS2" s="28"/>
-      <c r="BT2" s="28"/>
-      <c r="BU2" s="28"/>
-      <c r="BV2" s="27" t="s">
+      <c r="BS2" s="27"/>
+      <c r="BT2" s="27"/>
+      <c r="BU2" s="27"/>
+      <c r="BV2" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="BW2" s="28"/>
-      <c r="BX2" s="28"/>
-      <c r="BY2" s="28"/>
-      <c r="BZ2" s="27" t="s">
+      <c r="BW2" s="27"/>
+      <c r="BX2" s="27"/>
+      <c r="BY2" s="27"/>
+      <c r="BZ2" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="CA2" s="28"/>
-      <c r="CB2" s="28"/>
-      <c r="CC2" s="28"/>
-      <c r="CD2" s="28"/>
-      <c r="CE2" s="27" t="s">
+      <c r="CA2" s="27"/>
+      <c r="CB2" s="27"/>
+      <c r="CC2" s="27"/>
+      <c r="CD2" s="27"/>
+      <c r="CE2" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="CF2" s="28"/>
-      <c r="CG2" s="28"/>
-      <c r="CH2" s="28"/>
-      <c r="CI2" s="27" t="s">
+      <c r="CF2" s="27"/>
+      <c r="CG2" s="27"/>
+      <c r="CH2" s="27"/>
+      <c r="CI2" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="CJ2" s="28"/>
-      <c r="CK2" s="28"/>
-      <c r="CL2" s="28"/>
-      <c r="CM2" s="28"/>
-      <c r="CN2" s="27" t="s">
+      <c r="CJ2" s="27"/>
+      <c r="CK2" s="27"/>
+      <c r="CL2" s="27"/>
+      <c r="CM2" s="27"/>
+      <c r="CN2" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="CO2" s="28"/>
-      <c r="CP2" s="28"/>
-      <c r="CQ2" s="28"/>
-      <c r="CR2" s="27" t="s">
+      <c r="CO2" s="27"/>
+      <c r="CP2" s="27"/>
+      <c r="CQ2" s="27"/>
+      <c r="CR2" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="CS2" s="28"/>
-      <c r="CT2" s="28"/>
-      <c r="CU2" s="28"/>
-      <c r="CV2" s="27" t="s">
+      <c r="CS2" s="27"/>
+      <c r="CT2" s="27"/>
+      <c r="CU2" s="27"/>
+      <c r="CV2" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="CW2" s="28"/>
+      <c r="CW2" s="27"/>
       <c r="CX2" s="14">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:102" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="I3" s="4"/>
@@ -1459,7 +1603,7 @@
       <c r="P3" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="Q3" s="31" t="s">
+      <c r="Q3" s="29" t="s">
         <v>60</v>
       </c>
       <c r="R3" s="12" t="s">
@@ -1718,28 +1862,28 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:102" x14ac:dyDescent="0.3">
-      <c r="A4" s="23">
+    <row r="4" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="22">
         <v>1</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="24" t="s">
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="25">
+      <c r="I4" s="24">
         <v>44606</v>
       </c>
-      <c r="J4" s="25">
+      <c r="J4" s="24">
         <v>44606</v>
       </c>
-      <c r="K4" s="21"/>
+      <c r="K4" s="36"/>
       <c r="L4" s="19"/>
       <c r="M4" s="18"/>
       <c r="N4" s="19"/>
@@ -1754,10 +1898,10 @@
       <c r="W4" s="19"/>
       <c r="X4" s="19"/>
       <c r="Y4" s="19"/>
-      <c r="Z4" s="32" t="s">
+      <c r="Z4" s="18"/>
+      <c r="AA4" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="AA4" s="19"/>
       <c r="AB4" s="19"/>
       <c r="AC4" s="19"/>
       <c r="AD4" s="19"/>
@@ -1834,30 +1978,30 @@
       <c r="CW4" s="19"/>
       <c r="CX4" s="20"/>
     </row>
-    <row r="5" spans="1:102" x14ac:dyDescent="0.3">
-      <c r="A5" s="23">
+    <row r="5" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="22">
         <v>2</v>
       </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="24" t="s">
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="24" t="s">
+      <c r="H5" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="25">
+      <c r="I5" s="24">
         <v>44606</v>
       </c>
-      <c r="J5" s="25">
+      <c r="J5" s="24">
         <v>44620</v>
       </c>
-      <c r="K5" s="21"/>
-      <c r="L5" s="29"/>
-      <c r="M5" s="21"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="37"/>
       <c r="N5" s="19"/>
       <c r="O5" s="19"/>
       <c r="P5" s="19"/>
@@ -1870,10 +2014,10 @@
       <c r="W5" s="19"/>
       <c r="X5" s="19"/>
       <c r="Y5" s="19"/>
-      <c r="Z5" s="32" t="s">
+      <c r="Z5" s="18"/>
+      <c r="AA5" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="AA5" s="19"/>
       <c r="AB5" s="19"/>
       <c r="AC5" s="19"/>
       <c r="AD5" s="19"/>
@@ -1950,31 +2094,31 @@
       <c r="CW5" s="19"/>
       <c r="CX5" s="20"/>
     </row>
-    <row r="6" spans="1:102" x14ac:dyDescent="0.3">
-      <c r="A6" s="23">
+    <row r="6" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="22">
         <v>3</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="24" t="s">
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="H6" s="24" t="s">
+      <c r="H6" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="I6" s="25">
+      <c r="I6" s="24">
         <v>44620</v>
       </c>
-      <c r="J6" s="25">
+      <c r="J6" s="24">
         <v>44627</v>
       </c>
       <c r="K6" s="18"/>
       <c r="L6" s="19"/>
-      <c r="M6" s="21"/>
-      <c r="N6" s="29"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="38"/>
       <c r="O6" s="19"/>
       <c r="P6" s="19"/>
       <c r="Q6" s="19"/>
@@ -1986,10 +2130,10 @@
       <c r="W6" s="19"/>
       <c r="X6" s="19"/>
       <c r="Y6" s="19"/>
-      <c r="Z6" s="32" t="s">
+      <c r="Z6" s="18"/>
+      <c r="AA6" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="AA6" s="19"/>
       <c r="AB6" s="19"/>
       <c r="AC6" s="19"/>
       <c r="AD6" s="19"/>
@@ -2065,31 +2209,31 @@
       <c r="CV6" s="18"/>
       <c r="CW6" s="19"/>
     </row>
-    <row r="7" spans="1:102" x14ac:dyDescent="0.3">
-      <c r="A7" s="23">
+    <row r="7" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="22">
         <v>4</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="24" t="s">
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="H7" s="24" t="s">
+      <c r="H7" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="I7" s="25">
+      <c r="I7" s="24">
         <v>44627</v>
       </c>
-      <c r="J7" s="25">
+      <c r="J7" s="24">
         <v>44627</v>
       </c>
       <c r="K7" s="18"/>
       <c r="L7" s="19"/>
       <c r="M7" s="18"/>
-      <c r="N7" s="29"/>
+      <c r="N7" s="35"/>
       <c r="O7" s="19"/>
       <c r="P7" s="19"/>
       <c r="Q7" s="19"/>
@@ -2101,10 +2245,10 @@
       <c r="W7" s="19"/>
       <c r="X7" s="19"/>
       <c r="Y7" s="19"/>
-      <c r="Z7" s="32" t="s">
+      <c r="Z7" s="18"/>
+      <c r="AA7" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="AA7" s="19"/>
       <c r="AB7" s="19"/>
       <c r="AC7" s="19"/>
       <c r="AD7" s="19"/>
@@ -2180,25 +2324,25 @@
       <c r="CV7" s="18"/>
       <c r="CW7" s="19"/>
     </row>
-    <row r="8" spans="1:102" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="23">
+    <row r="8" spans="1:102" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="22">
         <v>24</v>
       </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="24" t="s">
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="H8" s="24" t="s">
+      <c r="H8" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="I8" s="25">
+      <c r="I8" s="24">
         <v>44638</v>
       </c>
-      <c r="J8" s="25">
+      <c r="J8" s="24">
         <v>44678</v>
       </c>
       <c r="K8" s="18"/>
@@ -2206,20 +2350,20 @@
       <c r="M8" s="18"/>
       <c r="N8" s="19"/>
       <c r="O8" s="19"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="29"/>
-      <c r="R8" s="21"/>
-      <c r="S8" s="29"/>
-      <c r="T8" s="29"/>
-      <c r="U8" s="29"/>
-      <c r="V8" s="18"/>
+      <c r="P8" s="31"/>
+      <c r="Q8" s="46"/>
+      <c r="R8" s="46"/>
+      <c r="S8" s="46"/>
+      <c r="T8" s="46"/>
+      <c r="U8" s="47"/>
+      <c r="V8" s="19"/>
       <c r="W8" s="19"/>
       <c r="X8" s="19"/>
       <c r="Y8" s="19"/>
-      <c r="Z8" s="32" t="s">
+      <c r="Z8" s="18"/>
+      <c r="AA8" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="AA8" s="19"/>
       <c r="AB8" s="19"/>
       <c r="AC8" s="19"/>
       <c r="AD8" s="19"/>
@@ -2295,25 +2439,25 @@
       <c r="CV8" s="18"/>
       <c r="CW8" s="19"/>
     </row>
-    <row r="9" spans="1:102" x14ac:dyDescent="0.3">
-      <c r="A9" s="23">
+    <row r="9" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="22">
         <v>6</v>
       </c>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="24" t="s">
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="H9" s="24" t="s">
+      <c r="H9" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="I9" s="25">
+      <c r="I9" s="24">
         <v>44650</v>
       </c>
-      <c r="J9" s="25">
+      <c r="J9" s="24">
         <v>44683</v>
       </c>
       <c r="K9" s="18"/>
@@ -2322,19 +2466,19 @@
       <c r="N9" s="19"/>
       <c r="O9" s="19"/>
       <c r="P9" s="19"/>
-      <c r="Q9" s="29"/>
-      <c r="R9" s="21"/>
-      <c r="S9" s="29"/>
-      <c r="T9" s="29"/>
-      <c r="U9" s="29"/>
-      <c r="V9" s="21"/>
+      <c r="Q9" s="31"/>
+      <c r="R9" s="32"/>
+      <c r="S9" s="33"/>
+      <c r="T9" s="33"/>
+      <c r="U9" s="33"/>
+      <c r="V9" s="34"/>
       <c r="W9" s="19"/>
       <c r="X9" s="19"/>
       <c r="Y9" s="19"/>
-      <c r="Z9" s="32" t="s">
+      <c r="Z9" s="18"/>
+      <c r="AA9" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="AA9" s="19"/>
       <c r="AB9" s="19"/>
       <c r="AC9" s="19"/>
       <c r="AD9" s="19"/>
@@ -2410,25 +2554,25 @@
       <c r="CV9" s="18"/>
       <c r="CW9" s="19"/>
     </row>
-    <row r="10" spans="1:102" x14ac:dyDescent="0.3">
-      <c r="A10" s="23">
+    <row r="10" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="22">
         <v>7</v>
       </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="24" t="s">
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="H10" s="24" t="s">
+      <c r="H10" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="I10" s="25">
+      <c r="I10" s="24">
         <v>44671</v>
       </c>
-      <c r="J10" s="25">
+      <c r="J10" s="24">
         <v>44683</v>
       </c>
       <c r="K10" s="18"/>
@@ -2440,16 +2584,16 @@
       <c r="Q10" s="19"/>
       <c r="R10" s="18"/>
       <c r="S10" s="19"/>
-      <c r="T10" s="29"/>
-      <c r="U10" s="29"/>
-      <c r="V10" s="21"/>
+      <c r="T10" s="31"/>
+      <c r="U10" s="33"/>
+      <c r="V10" s="34"/>
       <c r="W10" s="19"/>
       <c r="X10" s="19"/>
       <c r="Y10" s="19"/>
-      <c r="Z10" s="32" t="s">
+      <c r="Z10" s="18"/>
+      <c r="AA10" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="AA10" s="19"/>
       <c r="AB10" s="19"/>
       <c r="AC10" s="19"/>
       <c r="AD10" s="19"/>
@@ -2525,25 +2669,25 @@
       <c r="CV10" s="18"/>
       <c r="CW10" s="19"/>
     </row>
-    <row r="11" spans="1:102" x14ac:dyDescent="0.3">
-      <c r="A11" s="23">
+    <row r="11" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="22">
         <v>8</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="24" t="s">
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="H11" s="24" t="s">
+      <c r="H11" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="I11" s="25">
+      <c r="I11" s="24">
         <v>44684</v>
       </c>
-      <c r="J11" s="25">
+      <c r="J11" s="24">
         <v>44686</v>
       </c>
       <c r="K11" s="18"/>
@@ -2557,14 +2701,14 @@
       <c r="S11" s="19"/>
       <c r="T11" s="19"/>
       <c r="U11" s="19"/>
-      <c r="V11" s="21"/>
+      <c r="V11" s="35"/>
       <c r="W11" s="19"/>
       <c r="X11" s="19"/>
       <c r="Y11" s="19"/>
-      <c r="Z11" s="32" t="s">
+      <c r="Z11" s="18"/>
+      <c r="AA11" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="AA11" s="19"/>
       <c r="AB11" s="19"/>
       <c r="AC11" s="19"/>
       <c r="AD11" s="19"/>
@@ -2640,25 +2784,25 @@
       <c r="CV11" s="18"/>
       <c r="CW11" s="19"/>
     </row>
-    <row r="12" spans="1:102" x14ac:dyDescent="0.3">
-      <c r="A12" s="23">
+    <row r="12" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="22">
         <v>9</v>
       </c>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="24" t="s">
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="H12" s="24" t="s">
+      <c r="H12" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="I12" s="25">
+      <c r="I12" s="24">
         <v>44697</v>
       </c>
-      <c r="J12" s="25">
+      <c r="J12" s="24">
         <v>44697</v>
       </c>
       <c r="K12" s="18"/>
@@ -2674,12 +2818,12 @@
       <c r="U12" s="19"/>
       <c r="V12" s="18"/>
       <c r="W12" s="19"/>
-      <c r="X12" s="29"/>
+      <c r="X12" s="36"/>
       <c r="Y12" s="19"/>
-      <c r="Z12" s="32" t="s">
+      <c r="Z12" s="18"/>
+      <c r="AA12" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="AA12" s="19"/>
       <c r="AB12" s="19"/>
       <c r="AC12" s="19"/>
       <c r="AD12" s="19"/>
@@ -2755,25 +2899,27 @@
       <c r="CV12" s="18"/>
       <c r="CW12" s="19"/>
     </row>
-    <row r="13" spans="1:102" x14ac:dyDescent="0.3">
-      <c r="A13" s="23">
+    <row r="13" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="22">
         <v>19</v>
       </c>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="24" t="s">
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="H13" s="24" t="s">
+      <c r="H13" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="I13" s="25">
+      <c r="I13" s="24">
         <v>44698</v>
       </c>
-      <c r="J13" s="25"/>
+      <c r="J13" s="24">
+        <v>44728</v>
+      </c>
       <c r="K13" s="18"/>
       <c r="L13" s="19"/>
       <c r="M13" s="18"/>
@@ -2787,13 +2933,13 @@
       <c r="U13" s="19"/>
       <c r="V13" s="18"/>
       <c r="W13" s="19"/>
-      <c r="X13" s="36"/>
-      <c r="Y13" s="19"/>
-      <c r="Z13" s="32" t="s">
+      <c r="X13" s="39"/>
+      <c r="Y13" s="40"/>
+      <c r="Z13" s="41"/>
+      <c r="AA13" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="AA13" s="19"/>
-      <c r="AB13" s="19"/>
+      <c r="AB13" s="43"/>
       <c r="AC13" s="19"/>
       <c r="AD13" s="19"/>
       <c r="AE13" s="18"/>
@@ -2868,25 +3014,25 @@
       <c r="CV13" s="18"/>
       <c r="CW13" s="19"/>
     </row>
-    <row r="14" spans="1:102" x14ac:dyDescent="0.3">
-      <c r="A14" s="23">
+    <row r="14" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="22">
         <v>20</v>
       </c>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="24" t="s">
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="H14" s="24" t="s">
+      <c r="H14" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="I14" s="25">
+      <c r="I14" s="24">
         <v>44701</v>
       </c>
-      <c r="J14" s="25">
+      <c r="J14" s="24">
         <v>44716</v>
       </c>
       <c r="K14" s="18"/>
@@ -2903,11 +3049,11 @@
       <c r="V14" s="18"/>
       <c r="W14" s="19"/>
       <c r="X14" s="19"/>
-      <c r="Y14" s="29"/>
-      <c r="Z14" s="37" t="s">
+      <c r="Y14" s="31"/>
+      <c r="Z14" s="32"/>
+      <c r="AA14" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="AA14" s="29"/>
       <c r="AB14" s="19"/>
       <c r="AC14" s="19"/>
       <c r="AD14" s="19"/>
@@ -2983,25 +3129,25 @@
       <c r="CV14" s="18"/>
       <c r="CW14" s="19"/>
     </row>
-    <row r="15" spans="1:102" x14ac:dyDescent="0.3">
-      <c r="A15" s="23">
+    <row r="15" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="22">
         <v>12</v>
       </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="24" t="s">
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="H15" s="24" t="s">
+      <c r="H15" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="I15" s="25">
+      <c r="I15" s="24">
         <v>44714</v>
       </c>
-      <c r="J15" s="25">
+      <c r="J15" s="24">
         <v>44716</v>
       </c>
       <c r="K15" s="18"/>
@@ -3019,10 +3165,10 @@
       <c r="W15" s="19"/>
       <c r="X15" s="19"/>
       <c r="Y15" s="19"/>
-      <c r="Z15" s="37" t="s">
+      <c r="Z15" s="31"/>
+      <c r="AA15" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="AA15" s="29"/>
       <c r="AB15" s="19"/>
       <c r="AC15" s="19"/>
       <c r="AD15" s="19"/>
@@ -3098,25 +3244,25 @@
       <c r="CV15" s="18"/>
       <c r="CW15" s="19"/>
     </row>
-    <row r="16" spans="1:102" x14ac:dyDescent="0.3">
-      <c r="A16" s="23">
+    <row r="16" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="22">
         <v>13</v>
       </c>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="24" t="s">
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="H16" s="24" t="s">
+      <c r="H16" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="I16" s="25">
+      <c r="I16" s="24">
         <v>44704</v>
       </c>
-      <c r="J16" s="25"/>
+      <c r="J16" s="24"/>
       <c r="K16" s="18"/>
       <c r="L16" s="19"/>
       <c r="M16" s="18"/>
@@ -3131,11 +3277,11 @@
       <c r="V16" s="18"/>
       <c r="W16" s="19"/>
       <c r="X16" s="19"/>
-      <c r="Y16" s="36"/>
-      <c r="Z16" s="32" t="s">
+      <c r="Y16" s="45"/>
+      <c r="Z16" s="19"/>
+      <c r="AA16" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="AA16" s="19"/>
       <c r="AB16" s="19"/>
       <c r="AC16" s="19"/>
       <c r="AD16" s="19"/>
@@ -3211,23 +3357,23 @@
       <c r="CV16" s="18"/>
       <c r="CW16" s="19"/>
     </row>
-    <row r="17" spans="1:101" x14ac:dyDescent="0.3">
-      <c r="A17" s="23">
+    <row r="17" spans="1:101" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="22">
         <v>14</v>
       </c>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="24" t="s">
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="H17" s="24" t="s">
+      <c r="H17" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="I17" s="25"/>
-      <c r="J17" s="25"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
       <c r="K17" s="18"/>
       <c r="L17" s="19"/>
       <c r="M17" s="18"/>
@@ -3243,10 +3389,10 @@
       <c r="W17" s="19"/>
       <c r="X17" s="19"/>
       <c r="Y17" s="19"/>
-      <c r="Z17" s="32" t="s">
+      <c r="Z17" s="18"/>
+      <c r="AA17" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="AA17" s="19"/>
       <c r="AB17" s="19"/>
       <c r="AC17" s="19"/>
       <c r="AD17" s="19"/>
@@ -3322,43 +3468,47 @@
       <c r="CV17" s="18"/>
       <c r="CW17" s="19"/>
     </row>
-    <row r="18" spans="1:101" x14ac:dyDescent="0.3">
-      <c r="A18" s="23">
+    <row r="18" spans="1:101" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="22">
         <v>15</v>
       </c>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="4" t="s">
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="H18" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="I18" s="25"/>
-      <c r="J18" s="25"/>
+      <c r="H18" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="I18" s="24">
+        <v>44627</v>
+      </c>
+      <c r="J18" s="24">
+        <v>44728</v>
+      </c>
       <c r="K18" s="18"/>
       <c r="L18" s="19"/>
       <c r="M18" s="18"/>
-      <c r="N18" s="19"/>
-      <c r="O18" s="19"/>
-      <c r="P18" s="19"/>
-      <c r="Q18" s="19"/>
-      <c r="R18" s="18"/>
-      <c r="S18" s="19"/>
-      <c r="T18" s="19"/>
-      <c r="U18" s="19"/>
-      <c r="V18" s="18"/>
-      <c r="W18" s="19"/>
-      <c r="X18" s="19"/>
-      <c r="Y18" s="19"/>
-      <c r="Z18" s="32" t="s">
+      <c r="N18" s="39"/>
+      <c r="O18" s="40"/>
+      <c r="P18" s="40"/>
+      <c r="Q18" s="40"/>
+      <c r="R18" s="41"/>
+      <c r="S18" s="40"/>
+      <c r="T18" s="40"/>
+      <c r="U18" s="40"/>
+      <c r="V18" s="41"/>
+      <c r="W18" s="40"/>
+      <c r="X18" s="40"/>
+      <c r="Y18" s="40"/>
+      <c r="Z18" s="41"/>
+      <c r="AA18" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="AA18" s="19"/>
-      <c r="AB18" s="19"/>
+      <c r="AB18" s="43"/>
       <c r="AC18" s="19"/>
       <c r="AD18" s="19"/>
       <c r="AE18" s="18"/>
@@ -3434,22 +3584,16 @@
       <c r="CW18" s="19"/>
     </row>
     <row r="19" spans="1:101" x14ac:dyDescent="0.3">
-      <c r="A19" s="23">
-        <v>22</v>
-      </c>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="H19" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="I19" s="25"/>
-      <c r="J19" s="25"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
       <c r="K19" s="18"/>
       <c r="L19" s="19"/>
       <c r="M19" s="18"/>
@@ -3465,10 +3609,10 @@
       <c r="W19" s="19"/>
       <c r="X19" s="19"/>
       <c r="Y19" s="19"/>
-      <c r="Z19" s="32" t="s">
+      <c r="Z19" s="18"/>
+      <c r="AA19" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="AA19" s="19"/>
       <c r="AB19" s="19"/>
       <c r="AC19" s="19"/>
       <c r="AD19" s="19"/>
@@ -3545,47 +3689,33 @@
       <c r="CW19" s="19"/>
     </row>
     <row r="20" spans="1:101" x14ac:dyDescent="0.3">
-      <c r="A20" s="23">
-        <v>21</v>
-      </c>
-      <c r="B20" s="24"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="H20" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="I20" s="25">
-        <v>44627</v>
-      </c>
-      <c r="J20" s="25">
-        <v>44732</v>
-      </c>
+      <c r="A20" s="22"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="25"/>
       <c r="K20" s="18"/>
       <c r="L20" s="19"/>
       <c r="M20" s="18"/>
-      <c r="N20" s="33"/>
-      <c r="O20" s="33"/>
-      <c r="P20" s="33"/>
-      <c r="Q20" s="33"/>
-      <c r="R20" s="34"/>
-      <c r="S20" s="33"/>
-      <c r="T20" s="33"/>
-      <c r="U20" s="33"/>
-      <c r="V20" s="34"/>
-      <c r="W20" s="33"/>
-      <c r="X20" s="33"/>
-      <c r="Y20" s="33"/>
-      <c r="Z20" s="35" t="s">
+      <c r="N20" s="19"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="19"/>
+      <c r="Q20" s="19"/>
+      <c r="R20" s="18"/>
+      <c r="S20" s="19"/>
+      <c r="T20" s="19"/>
+      <c r="U20" s="19"/>
+      <c r="V20" s="18"/>
+      <c r="W20" s="19"/>
+      <c r="X20" s="19"/>
+      <c r="Y20" s="19"/>
+      <c r="Z20" s="18"/>
+      <c r="AA20" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="AA20" s="33"/>
-      <c r="AB20" s="33"/>
-      <c r="AC20" s="33"/>
+      <c r="AB20" s="19"/>
+      <c r="AC20" s="19"/>
       <c r="AD20" s="19"/>
       <c r="AE20" s="18"/>
       <c r="AF20" s="19"/>
@@ -3660,24 +3790,24 @@
       <c r="CW20" s="19"/>
     </row>
     <row r="21" spans="1:101" x14ac:dyDescent="0.3">
-      <c r="A21" s="23"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="26"/>
+      <c r="A21" s="22"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="25"/>
     </row>
     <row r="22" spans="1:101" x14ac:dyDescent="0.3">
-      <c r="A22" s="23"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="25"/>
-      <c r="J22" s="25"/>
+      <c r="A22" s="22"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>

</xml_diff>

<commit_message>
Ajout de fonctionnalité manquante
</commit_message>
<xml_diff>
--- a/GPI/GANTT.xlsx
+++ b/GPI/GANTT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\iut\G4S2\SAE\GRAMA - git\GPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D3E935-3424-4E89-912D-7DFF851CC332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF71BF8-CABA-4903-A43C-0375651911DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{E5182A25-CAA6-4D67-9071-9F4C8FE9A0AC}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="117">
   <si>
     <t>WBS</t>
   </si>
@@ -506,7 +506,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -541,137 +541,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -733,55 +607,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1224,7 +1065,7 @@
       <selection activeCell="G1" sqref="G1"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
-      <selection pane="bottomRight" activeCell="Y5" sqref="Y5"/>
+      <selection pane="bottomRight" activeCell="AE21" sqref="AE21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1580,7 +1421,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:102" x14ac:dyDescent="0.3">
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="I3" s="4"/>
@@ -1862,7 +1703,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A4" s="22">
         <v>1</v>
       </c>
@@ -1883,7 +1724,7 @@
       <c r="J4" s="24">
         <v>44606</v>
       </c>
-      <c r="K4" s="36"/>
+      <c r="K4" s="31"/>
       <c r="L4" s="19"/>
       <c r="M4" s="18"/>
       <c r="N4" s="19"/>
@@ -1978,7 +1819,7 @@
       <c r="CW4" s="19"/>
       <c r="CX4" s="20"/>
     </row>
-    <row r="5" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A5" s="22">
         <v>2</v>
       </c>
@@ -2000,8 +1841,8 @@
         <v>44620</v>
       </c>
       <c r="K5" s="31"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="37"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="31"/>
       <c r="N5" s="19"/>
       <c r="O5" s="19"/>
       <c r="P5" s="19"/>
@@ -2094,7 +1935,7 @@
       <c r="CW5" s="19"/>
       <c r="CX5" s="20"/>
     </row>
-    <row r="6" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A6" s="22">
         <v>3</v>
       </c>
@@ -2118,7 +1959,7 @@
       <c r="K6" s="18"/>
       <c r="L6" s="19"/>
       <c r="M6" s="31"/>
-      <c r="N6" s="38"/>
+      <c r="N6" s="32"/>
       <c r="O6" s="19"/>
       <c r="P6" s="19"/>
       <c r="Q6" s="19"/>
@@ -2209,7 +2050,7 @@
       <c r="CV6" s="18"/>
       <c r="CW6" s="19"/>
     </row>
-    <row r="7" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A7" s="22">
         <v>4</v>
       </c>
@@ -2233,7 +2074,7 @@
       <c r="K7" s="18"/>
       <c r="L7" s="19"/>
       <c r="M7" s="18"/>
-      <c r="N7" s="35"/>
+      <c r="N7" s="32"/>
       <c r="O7" s="19"/>
       <c r="P7" s="19"/>
       <c r="Q7" s="19"/>
@@ -2324,7 +2165,7 @@
       <c r="CV7" s="18"/>
       <c r="CW7" s="19"/>
     </row>
-    <row r="8" spans="1:102" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:102" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="22">
         <v>24</v>
       </c>
@@ -2350,13 +2191,13 @@
       <c r="M8" s="18"/>
       <c r="N8" s="19"/>
       <c r="O8" s="19"/>
-      <c r="P8" s="31"/>
-      <c r="Q8" s="46"/>
-      <c r="R8" s="46"/>
-      <c r="S8" s="46"/>
-      <c r="T8" s="46"/>
-      <c r="U8" s="47"/>
-      <c r="V8" s="19"/>
+      <c r="P8" s="32"/>
+      <c r="Q8" s="32"/>
+      <c r="R8" s="31"/>
+      <c r="S8" s="32"/>
+      <c r="T8" s="32"/>
+      <c r="U8" s="32"/>
+      <c r="V8" s="18"/>
       <c r="W8" s="19"/>
       <c r="X8" s="19"/>
       <c r="Y8" s="19"/>
@@ -2439,7 +2280,7 @@
       <c r="CV8" s="18"/>
       <c r="CW8" s="19"/>
     </row>
-    <row r="9" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A9" s="22">
         <v>6</v>
       </c>
@@ -2466,12 +2307,12 @@
       <c r="N9" s="19"/>
       <c r="O9" s="19"/>
       <c r="P9" s="19"/>
-      <c r="Q9" s="31"/>
-      <c r="R9" s="32"/>
-      <c r="S9" s="33"/>
-      <c r="T9" s="33"/>
-      <c r="U9" s="33"/>
-      <c r="V9" s="34"/>
+      <c r="Q9" s="32"/>
+      <c r="R9" s="31"/>
+      <c r="S9" s="32"/>
+      <c r="T9" s="32"/>
+      <c r="U9" s="32"/>
+      <c r="V9" s="31"/>
       <c r="W9" s="19"/>
       <c r="X9" s="19"/>
       <c r="Y9" s="19"/>
@@ -2554,7 +2395,7 @@
       <c r="CV9" s="18"/>
       <c r="CW9" s="19"/>
     </row>
-    <row r="10" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A10" s="22">
         <v>7</v>
       </c>
@@ -2584,9 +2425,9 @@
       <c r="Q10" s="19"/>
       <c r="R10" s="18"/>
       <c r="S10" s="19"/>
-      <c r="T10" s="31"/>
-      <c r="U10" s="33"/>
-      <c r="V10" s="34"/>
+      <c r="T10" s="32"/>
+      <c r="U10" s="32"/>
+      <c r="V10" s="31"/>
       <c r="W10" s="19"/>
       <c r="X10" s="19"/>
       <c r="Y10" s="19"/>
@@ -2669,7 +2510,7 @@
       <c r="CV10" s="18"/>
       <c r="CW10" s="19"/>
     </row>
-    <row r="11" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A11" s="22">
         <v>8</v>
       </c>
@@ -2701,7 +2542,7 @@
       <c r="S11" s="19"/>
       <c r="T11" s="19"/>
       <c r="U11" s="19"/>
-      <c r="V11" s="35"/>
+      <c r="V11" s="31"/>
       <c r="W11" s="19"/>
       <c r="X11" s="19"/>
       <c r="Y11" s="19"/>
@@ -2784,7 +2625,7 @@
       <c r="CV11" s="18"/>
       <c r="CW11" s="19"/>
     </row>
-    <row r="12" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A12" s="22">
         <v>9</v>
       </c>
@@ -2818,7 +2659,7 @@
       <c r="U12" s="19"/>
       <c r="V12" s="18"/>
       <c r="W12" s="19"/>
-      <c r="X12" s="36"/>
+      <c r="X12" s="32"/>
       <c r="Y12" s="19"/>
       <c r="Z12" s="18"/>
       <c r="AA12" s="30" t="s">
@@ -2899,7 +2740,7 @@
       <c r="CV12" s="18"/>
       <c r="CW12" s="19"/>
     </row>
-    <row r="13" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A13" s="22">
         <v>19</v>
       </c>
@@ -2933,13 +2774,13 @@
       <c r="U13" s="19"/>
       <c r="V13" s="18"/>
       <c r="W13" s="19"/>
-      <c r="X13" s="39"/>
-      <c r="Y13" s="40"/>
-      <c r="Z13" s="41"/>
-      <c r="AA13" s="42" t="s">
+      <c r="X13" s="34"/>
+      <c r="Y13" s="34"/>
+      <c r="Z13" s="35"/>
+      <c r="AA13" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="AB13" s="43"/>
+      <c r="AB13" s="34"/>
       <c r="AC13" s="19"/>
       <c r="AD13" s="19"/>
       <c r="AE13" s="18"/>
@@ -3014,7 +2855,7 @@
       <c r="CV13" s="18"/>
       <c r="CW13" s="19"/>
     </row>
-    <row r="14" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A14" s="22">
         <v>20</v>
       </c>
@@ -3049,9 +2890,9 @@
       <c r="V14" s="18"/>
       <c r="W14" s="19"/>
       <c r="X14" s="19"/>
-      <c r="Y14" s="31"/>
-      <c r="Z14" s="32"/>
-      <c r="AA14" s="44" t="s">
+      <c r="Y14" s="32"/>
+      <c r="Z14" s="31"/>
+      <c r="AA14" s="33" t="s">
         <v>13</v>
       </c>
       <c r="AB14" s="19"/>
@@ -3129,7 +2970,7 @@
       <c r="CV14" s="18"/>
       <c r="CW14" s="19"/>
     </row>
-    <row r="15" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A15" s="22">
         <v>12</v>
       </c>
@@ -3166,7 +3007,7 @@
       <c r="X15" s="19"/>
       <c r="Y15" s="19"/>
       <c r="Z15" s="31"/>
-      <c r="AA15" s="44" t="s">
+      <c r="AA15" s="33" t="s">
         <v>13</v>
       </c>
       <c r="AB15" s="19"/>
@@ -3244,7 +3085,7 @@
       <c r="CV15" s="18"/>
       <c r="CW15" s="19"/>
     </row>
-    <row r="16" spans="1:102" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:102" x14ac:dyDescent="0.3">
       <c r="A16" s="22">
         <v>13</v>
       </c>
@@ -3262,7 +3103,9 @@
       <c r="I16" s="24">
         <v>44704</v>
       </c>
-      <c r="J16" s="24"/>
+      <c r="J16" s="24">
+        <v>44728</v>
+      </c>
       <c r="K16" s="18"/>
       <c r="L16" s="19"/>
       <c r="M16" s="18"/>
@@ -3277,12 +3120,12 @@
       <c r="V16" s="18"/>
       <c r="W16" s="19"/>
       <c r="X16" s="19"/>
-      <c r="Y16" s="45"/>
-      <c r="Z16" s="19"/>
-      <c r="AA16" s="30" t="s">
+      <c r="Y16" s="34"/>
+      <c r="Z16" s="35"/>
+      <c r="AA16" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="AB16" s="19"/>
+      <c r="AB16" s="34"/>
       <c r="AC16" s="19"/>
       <c r="AD16" s="19"/>
       <c r="AE16" s="18"/>
@@ -3357,7 +3200,7 @@
       <c r="CV16" s="18"/>
       <c r="CW16" s="19"/>
     </row>
-    <row r="17" spans="1:101" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A17" s="22">
         <v>14</v>
       </c>
@@ -3372,8 +3215,12 @@
       <c r="H17" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="I17" s="24"/>
-      <c r="J17" s="24"/>
+      <c r="I17" s="24">
+        <v>44725</v>
+      </c>
+      <c r="J17" s="24">
+        <v>44728</v>
+      </c>
       <c r="K17" s="18"/>
       <c r="L17" s="19"/>
       <c r="M17" s="18"/>
@@ -3393,7 +3240,7 @@
       <c r="AA17" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="AB17" s="19"/>
+      <c r="AB17" s="34"/>
       <c r="AC17" s="19"/>
       <c r="AD17" s="19"/>
       <c r="AE17" s="18"/>
@@ -3468,7 +3315,7 @@
       <c r="CV17" s="18"/>
       <c r="CW17" s="19"/>
     </row>
-    <row r="18" spans="1:101" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A18" s="22">
         <v>15</v>
       </c>
@@ -3492,23 +3339,23 @@
       <c r="K18" s="18"/>
       <c r="L18" s="19"/>
       <c r="M18" s="18"/>
-      <c r="N18" s="39"/>
-      <c r="O18" s="40"/>
-      <c r="P18" s="40"/>
-      <c r="Q18" s="40"/>
-      <c r="R18" s="41"/>
-      <c r="S18" s="40"/>
-      <c r="T18" s="40"/>
-      <c r="U18" s="40"/>
-      <c r="V18" s="41"/>
-      <c r="W18" s="40"/>
-      <c r="X18" s="40"/>
-      <c r="Y18" s="40"/>
-      <c r="Z18" s="41"/>
-      <c r="AA18" s="42" t="s">
+      <c r="N18" s="34"/>
+      <c r="O18" s="34"/>
+      <c r="P18" s="34"/>
+      <c r="Q18" s="34"/>
+      <c r="R18" s="35"/>
+      <c r="S18" s="34"/>
+      <c r="T18" s="34"/>
+      <c r="U18" s="34"/>
+      <c r="V18" s="35"/>
+      <c r="W18" s="34"/>
+      <c r="X18" s="34"/>
+      <c r="Y18" s="34"/>
+      <c r="Z18" s="35"/>
+      <c r="AA18" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="AB18" s="43"/>
+      <c r="AB18" s="34"/>
       <c r="AC18" s="19"/>
       <c r="AD18" s="19"/>
       <c r="AE18" s="18"/>
@@ -3594,99 +3441,6 @@
       <c r="H19" s="23"/>
       <c r="I19" s="24"/>
       <c r="J19" s="24"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="19"/>
-      <c r="M19" s="18"/>
-      <c r="N19" s="19"/>
-      <c r="O19" s="19"/>
-      <c r="P19" s="19"/>
-      <c r="Q19" s="19"/>
-      <c r="R19" s="18"/>
-      <c r="S19" s="19"/>
-      <c r="T19" s="19"/>
-      <c r="U19" s="19"/>
-      <c r="V19" s="18"/>
-      <c r="W19" s="19"/>
-      <c r="X19" s="19"/>
-      <c r="Y19" s="19"/>
-      <c r="Z19" s="18"/>
-      <c r="AA19" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB19" s="19"/>
-      <c r="AC19" s="19"/>
-      <c r="AD19" s="19"/>
-      <c r="AE19" s="18"/>
-      <c r="AF19" s="19"/>
-      <c r="AG19" s="19"/>
-      <c r="AH19" s="19"/>
-      <c r="AI19" s="18"/>
-      <c r="AJ19" s="19"/>
-      <c r="AK19" s="19"/>
-      <c r="AL19" s="19"/>
-      <c r="AM19" s="18"/>
-      <c r="AN19" s="19"/>
-      <c r="AO19" s="19"/>
-      <c r="AP19" s="19"/>
-      <c r="AQ19" s="19"/>
-      <c r="AR19" s="18"/>
-      <c r="AS19" s="19"/>
-      <c r="AT19" s="19"/>
-      <c r="AU19" s="19"/>
-      <c r="AV19" s="18"/>
-      <c r="AW19" s="19"/>
-      <c r="AX19" s="19"/>
-      <c r="AY19" s="19"/>
-      <c r="AZ19" s="18"/>
-      <c r="BA19" s="19"/>
-      <c r="BB19" s="19"/>
-      <c r="BC19" s="19"/>
-      <c r="BD19" s="19"/>
-      <c r="BE19" s="18"/>
-      <c r="BF19" s="19"/>
-      <c r="BG19" s="19"/>
-      <c r="BH19" s="19"/>
-      <c r="BI19" s="18"/>
-      <c r="BJ19" s="19"/>
-      <c r="BK19" s="19"/>
-      <c r="BL19" s="19"/>
-      <c r="BM19" s="18"/>
-      <c r="BN19" s="19"/>
-      <c r="BO19" s="19"/>
-      <c r="BP19" s="19"/>
-      <c r="BQ19" s="19"/>
-      <c r="BR19" s="18"/>
-      <c r="BS19" s="19"/>
-      <c r="BT19" s="19"/>
-      <c r="BU19" s="19"/>
-      <c r="BV19" s="18"/>
-      <c r="BW19" s="19"/>
-      <c r="BX19" s="19"/>
-      <c r="BY19" s="19"/>
-      <c r="BZ19" s="18"/>
-      <c r="CA19" s="19"/>
-      <c r="CB19" s="19"/>
-      <c r="CC19" s="19"/>
-      <c r="CD19" s="19"/>
-      <c r="CE19" s="18"/>
-      <c r="CF19" s="19"/>
-      <c r="CG19" s="19"/>
-      <c r="CH19" s="19"/>
-      <c r="CI19" s="18"/>
-      <c r="CJ19" s="19"/>
-      <c r="CK19" s="19"/>
-      <c r="CL19" s="19"/>
-      <c r="CM19" s="19"/>
-      <c r="CN19" s="18"/>
-      <c r="CO19" s="19"/>
-      <c r="CP19" s="19"/>
-      <c r="CQ19" s="19"/>
-      <c r="CR19" s="18"/>
-      <c r="CS19" s="19"/>
-      <c r="CT19" s="19"/>
-      <c r="CU19" s="19"/>
-      <c r="CV19" s="18"/>
-      <c r="CW19" s="19"/>
     </row>
     <row r="20" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A20" s="22"/>
@@ -3695,99 +3449,6 @@
       <c r="D20" s="24"/>
       <c r="E20" s="24"/>
       <c r="F20" s="25"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="19"/>
-      <c r="M20" s="18"/>
-      <c r="N20" s="19"/>
-      <c r="O20" s="19"/>
-      <c r="P20" s="19"/>
-      <c r="Q20" s="19"/>
-      <c r="R20" s="18"/>
-      <c r="S20" s="19"/>
-      <c r="T20" s="19"/>
-      <c r="U20" s="19"/>
-      <c r="V20" s="18"/>
-      <c r="W20" s="19"/>
-      <c r="X20" s="19"/>
-      <c r="Y20" s="19"/>
-      <c r="Z20" s="18"/>
-      <c r="AA20" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB20" s="19"/>
-      <c r="AC20" s="19"/>
-      <c r="AD20" s="19"/>
-      <c r="AE20" s="18"/>
-      <c r="AF20" s="19"/>
-      <c r="AG20" s="19"/>
-      <c r="AH20" s="19"/>
-      <c r="AI20" s="18"/>
-      <c r="AJ20" s="19"/>
-      <c r="AK20" s="19"/>
-      <c r="AL20" s="19"/>
-      <c r="AM20" s="18"/>
-      <c r="AN20" s="19"/>
-      <c r="AO20" s="19"/>
-      <c r="AP20" s="19"/>
-      <c r="AQ20" s="19"/>
-      <c r="AR20" s="18"/>
-      <c r="AS20" s="19"/>
-      <c r="AT20" s="19"/>
-      <c r="AU20" s="19"/>
-      <c r="AV20" s="18"/>
-      <c r="AW20" s="19"/>
-      <c r="AX20" s="19"/>
-      <c r="AY20" s="19"/>
-      <c r="AZ20" s="18"/>
-      <c r="BA20" s="19"/>
-      <c r="BB20" s="19"/>
-      <c r="BC20" s="19"/>
-      <c r="BD20" s="19"/>
-      <c r="BE20" s="18"/>
-      <c r="BF20" s="19"/>
-      <c r="BG20" s="19"/>
-      <c r="BH20" s="19"/>
-      <c r="BI20" s="18"/>
-      <c r="BJ20" s="19"/>
-      <c r="BK20" s="19"/>
-      <c r="BL20" s="19"/>
-      <c r="BM20" s="18"/>
-      <c r="BN20" s="19"/>
-      <c r="BO20" s="19"/>
-      <c r="BP20" s="19"/>
-      <c r="BQ20" s="19"/>
-      <c r="BR20" s="18"/>
-      <c r="BS20" s="19"/>
-      <c r="BT20" s="19"/>
-      <c r="BU20" s="19"/>
-      <c r="BV20" s="18"/>
-      <c r="BW20" s="19"/>
-      <c r="BX20" s="19"/>
-      <c r="BY20" s="19"/>
-      <c r="BZ20" s="18"/>
-      <c r="CA20" s="19"/>
-      <c r="CB20" s="19"/>
-      <c r="CC20" s="19"/>
-      <c r="CD20" s="19"/>
-      <c r="CE20" s="18"/>
-      <c r="CF20" s="19"/>
-      <c r="CG20" s="19"/>
-      <c r="CH20" s="19"/>
-      <c r="CI20" s="18"/>
-      <c r="CJ20" s="19"/>
-      <c r="CK20" s="19"/>
-      <c r="CL20" s="19"/>
-      <c r="CM20" s="19"/>
-      <c r="CN20" s="18"/>
-      <c r="CO20" s="19"/>
-      <c r="CP20" s="19"/>
-      <c r="CQ20" s="19"/>
-      <c r="CR20" s="18"/>
-      <c r="CS20" s="19"/>
-      <c r="CT20" s="19"/>
-      <c r="CU20" s="19"/>
-      <c r="CV20" s="18"/>
-      <c r="CW20" s="19"/>
     </row>
     <row r="21" spans="1:101" x14ac:dyDescent="0.3">
       <c r="A21" s="22"/>

</xml_diff>